<commit_message>
Revisão pontual no modo MONITOR, inserindo consulta à lista global de exceções.
</commit_message>
<xml_diff>
--- a/Settings/monitorGeral.xlsx
+++ b/Settings/monitorGeral.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="446">
   <si>
     <t xml:space="preserve">Registro </t>
   </si>
@@ -561,6 +561,849 @@
   </si>
   <si>
     <t>30/09/2022 13:15:00</t>
+  </si>
+  <si>
+    <t>RFeye002289</t>
+  </si>
+  <si>
+    <t>RFeye002177</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>[DOC] CH06 VHF, Segurança/socorro</t>
+  </si>
+  <si>
+    <t>[AISW] SBSV-RDONAV, VOR/DME SVD, Deputado Luís Eduardo Magalhães</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (50415723132, 1007661442), Salvador/BA | [ICAO] ATIS B-260/450, SALVADOR | [AISW] SBSV-COM, ATIS, Deputado Luís Eduardo Magalhães</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478453), Fortaleza/CE | [ICAO] ATIS B-260/450, FORTALEZA | [AISW] SBFZ-COM, ATIS, Pinto Martins</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>RFeye002289</t>
+  </si>
+  <si>
+    <t>{"Bands":[{"FreqStart":108000,"FreqStop":137000}],"Contour":30,"GarbageMask":["mask_Channels.csv","mask_80dBm.csv"]}</t>
+  </si>
+  <si>
+    <t>matlab.io.ftp.FTP (201.45.154.242:0)
+EMISSÕES DESMASCARADAS ([MHz, kHz]): [[111.9,76],[116.5,100],[127.75,76]]</t>
+  </si>
+  <si>
+    <t>01/12/2022 11:27:14</t>
+  </si>
+  <si>
+    <t>01/12/2022 11:30:52</t>
+  </si>
+  <si>
+    <t>RFeye002289</t>
+  </si>
+  <si>
+    <t>RFeye002177</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>[DOC] CH06 VHF, Segurança/socorro</t>
+  </si>
+  <si>
+    <t>[AISW] SBSV-RDONAV, VOR/DME SVD, Deputado Luís Eduardo Magalhães</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (50415723132, 1007661442), Salvador/BA | [ICAO] ATIS B-260/450, SALVADOR | [AISW] SBSV-COM, ATIS, Deputado Luís Eduardo Magalhães</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478453), Fortaleza/CE | [ICAO] ATIS B-260/450, FORTALEZA | [AISW] SBFZ-COM, ATIS, Pinto Martins</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>RFeye002289</t>
+  </si>
+  <si>
+    <t>{"Bands":[{"FreqStart":108000,"FreqStop":137000}],"Contour":30,"GarbageMask":["mask_Channels.csv","mask_80dBm.csv"]}</t>
+  </si>
+  <si>
+    <t>matlab.io.ftp.FTP (201.45.154.242:0)
+EMISSÕES DESMASCARADAS ([MHz, kHz]): [[111.9,76],[116.5,100],[127.75,76]]</t>
+  </si>
+  <si>
+    <t>01/12/2022 11:31:53</t>
+  </si>
+  <si>
+    <t>01/12/2022 11:32:06</t>
+  </si>
+  <si>
+    <t>RFeye002289</t>
+  </si>
+  <si>
+    <t>RFeye002177</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[AISW] SBSV-RDONAV, VOR/DME SVD, Deputado Luís Eduardo Magalhães</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (50415723132, 1007661442), Salvador/BA | [ICAO] ATIS B-260/450, SALVADOR | [AISW] SBSV-COM, ATIS, Deputado Luís Eduardo Magalhães</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478453), Fortaleza/CE | [ICAO] ATIS B-260/450, FORTALEZA | [AISW] SBFZ-COM, ATIS, Pinto Martins</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>RFeye002289</t>
+  </si>
+  <si>
+    <t>{"Bands":[{"FreqStart":108000,"FreqStop":137000}],"Contour":30,"GarbageMask":["mask_Channels.csv","mask_80dBm.csv"]}</t>
+  </si>
+  <si>
+    <t>matlab.io.ftp.FTP (201.45.154.242:0)
+EMISSÕES DESMASCARADAS ([MHz, kHz]): [[111.9,76],[116.5,100],[127.75,76]]</t>
+  </si>
+  <si>
+    <t>01/12/2022 11:32:22</t>
+  </si>
+  <si>
+    <t>01/12/2022 11:32:34</t>
+  </si>
+  <si>
+    <t>RFeye002177</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>[MOS] FM-C2, A4, Fundacao Cearense De Pesquisa E Cultura (10008000590, 322869790), Fortaleza/CE</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (50415723132, 1006703370), Fortaleza/CE</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478453), Fortaleza/CE | [ICAO] TWR 25/40, FORTALEZA | [AISW] SBFZ-COM, TORRE, Pinto Martins</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478453), Fortaleza/CE | [ICAO] APP-U C-150/450, FORTALEZA</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478453), Fortaleza/CE | [ICAO] ACC-U C-261/450, FORTALEZA</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>RFeye002289</t>
+  </si>
+  <si>
+    <t>{"Contour":30,"GarbageMask":["mask_Channels.csv","mask_80dBm.csv"],"Persistent":{"ThreadIDList":310,"BrokenMsg":5,"ScansPerMinute":60,"THR1_Global":30,"THR2_OCC":0.1}}</t>
+  </si>
+  <si>
+    <t>matlab.io.ftp.FTP (201.45.154.242:0)
+Não recebidos datagramas do sensor RFeye002289</t>
+  </si>
+  <si>
+    <t>01/12/2022 11:32:43</t>
+  </si>
+  <si>
+    <t>01/12/2022 11:33:11</t>
+  </si>
+  <si>
+    <t>RFeye002289</t>
+  </si>
+  <si>
+    <t>RFeye002177</t>
+  </si>
+  <si>
+    <t>RFeye002159</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[AISW] SBSV-RDONAV, VOR/DME SVD, Deputado Luís Eduardo Magalhães</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (50415723132, 1007661442), Salvador/BA | [ICAO] ATIS B-260/450, SALVADOR | [AISW] SBSV-COM, ATIS, Deputado Luís Eduardo Magalhães</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478453), Fortaleza/CE | [ICAO] ATIS B-260/450, FORTALEZA | [AISW] SBFZ-COM, ATIS, Pinto Martins</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>RFeye002159</t>
+  </si>
+  <si>
+    <t>{"Bands":[{"FreqStart":108000,"FreqStop":137000}],"Contour":30,"GarbageMask":["mask_Channels.csv","mask_80dBm.csv"]}</t>
+  </si>
+  <si>
+    <t>matlab.io.ftp.FTP (200.254.11.114:0)
+EMISSÕES DESMASCARADAS ([MHz, kHz]): [127.65,50]</t>
+  </si>
+  <si>
+    <t>01/12/2022 11:33:58</t>
+  </si>
+  <si>
+    <t>01/12/2022 11:35:29</t>
+  </si>
+  <si>
+    <t>RFeye002177</t>
+  </si>
+  <si>
+    <t>RFeye002159</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>[MOS] FM-C2, A4, Fundacao Cearense De Pesquisa E Cultura (10008000590, 322869790), Fortaleza/CE</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (50415723132, 1006703370), Fortaleza/CE</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478453), Fortaleza/CE | [ICAO] TWR 25/40, FORTALEZA | [AISW] SBFZ-COM, TORRE, Pinto Martins</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478453), Fortaleza/CE | [ICAO] APP-U C-150/450, FORTALEZA</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478453), Fortaleza/CE | [ICAO] ACC-U C-261/450, FORTALEZA</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478402), Porto Seguro/BA | [ICAO] ACC-U C-261/450, PORTO SEGURO</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (50415723132, 1007661469), Porto Seguro/BA | [ICAO] ACC-U C-261/450, PORTO SEGURO</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>RFeye002159</t>
+  </si>
+  <si>
+    <t>{"Contour":30,"GarbageMask":["mask_Channels.csv","mask_80dBm.csv"],"Persistent":{"ThreadIDList":310,"BrokenMsg":5,"ScansPerMinute":60,"THR1_Global":30,"THR2_OCC":0.1}}</t>
+  </si>
+  <si>
+    <t>matlab.io.ftp.FTP (200.254.11.114:0)
+CONTADOR MÉDIO DE ROMPIMENTO DE MÁSCARA:
+{"beginTime":"01/12/2022 14:38:00","endTime":"01/12/2022 14:44:00","countBroken_Mean":[[300,0],[310,32],[320,0],[330,0],[340,0],[350,1],[360,0],[370,7],[380,0],[390,0]]}
+EMISSÕES PERSISTENTES ([MHz, kHz]): [[123.794,49],[125.084,49],[125.982,49],[128.337,59],[133.006,49],[135.282,59],[135.643,59]]</t>
+  </si>
+  <si>
+    <t>01/12/2022 11:36:00</t>
+  </si>
+  <si>
+    <t>01/12/2022 11:44:01</t>
+  </si>
+  <si>
+    <t>RFeye002177</t>
+  </si>
+  <si>
+    <t>RFeye002159</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>[MOS] FM-C2, A4, Fundacao Cearense De Pesquisa E Cultura (10008000590, 322869790), Fortaleza/CE</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (50415723132, 1006703370), Fortaleza/CE</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478453), Fortaleza/CE | [ICAO] TWR 25/40, FORTALEZA | [AISW] SBFZ-COM, TORRE, Pinto Martins</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478453), Fortaleza/CE | [ICAO] APP-U C-150/450, FORTALEZA</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478453), Fortaleza/CE | [ICAO] ACC-U C-261/450, FORTALEZA</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478402), Porto Seguro/BA | [ICAO] ACC-U C-261/450, PORTO SEGURO</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (50415723132, 1007661469), Porto Seguro/BA | [ICAO] ACC-U C-261/450, PORTO SEGURO</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478402), Porto Seguro/BA | [ICAO] ACC-U C-261/450, PORTO SEGURO</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>RFeye002159</t>
+  </si>
+  <si>
+    <t>{"Contour":30,"GarbageMask":["mask_Channels.csv","mask_80dBm.csv"],"Persistent":{"ThreadIDList":310,"BrokenMsg":5,"ScansPerMinute":60,"THR1_Global":30,"THR2_OCC":0.1}}</t>
+  </si>
+  <si>
+    <t>matlab.io.ftp.FTP (200.254.11.114:0)
+CONTADOR MÉDIO DE ROMPIMENTO DE MÁSCARA:
+{"beginTime":"01/12/2022 14:50:00","endTime":"01/12/2022 14:55:00","countBroken_Mean":[[300,0],[310,31],[320,0],[330,0],[340,0],[350,1],[360,1],[370,8],[380,0],[390,0]]}
+EMISSÕES PERSISTENTES ([MHz, kHz]): [[122.817,49],[123.794,49],[125.093,49],[125.982,49],[128.337,49],[133.016,49],[135.282,59],[135.634,59]]</t>
+  </si>
+  <si>
+    <t>01/12/2022 11:46:36</t>
+  </si>
+  <si>
+    <t>01/12/2022 11:55:01</t>
+  </si>
+  <si>
+    <t>RFeye002289</t>
+  </si>
+  <si>
+    <t>RFeye002177</t>
+  </si>
+  <si>
+    <t>RFeye002159</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[AISW] SBSV-RDONAV, VOR/DME SVD, Deputado Luís Eduardo Magalhães</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (50415723132, 1007661442), Salvador/BA | [ICAO] ATIS B-260/450, SALVADOR | [AISW] SBSV-COM, ATIS, Deputado Luís Eduardo Magalhães</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478453), Fortaleza/CE | [ICAO] ATIS B-260/450, FORTALEZA | [AISW] SBFZ-COM, ATIS, Pinto Martins</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>RFeye002289</t>
+  </si>
+  <si>
+    <t>{"Bands":[{"FreqStart":108000,"FreqStop":137000}],"Contour":30,"GarbageMask":["mask_Channels.csv","mask_80dBm.csv"]}</t>
+  </si>
+  <si>
+    <t>matlab.io.ftp.FTP (201.45.154.242:0)
+EMISSÕES DESMASCARADAS ([MHz, kHz]): [[111.9,76],[116.5,100],[127.75,76]]</t>
+  </si>
+  <si>
+    <t>01/12/2022 11:57:56</t>
+  </si>
+  <si>
+    <t>01/12/2022 11:58:11</t>
+  </si>
+  <si>
+    <t>RFeye002177</t>
+  </si>
+  <si>
+    <t>RFeye002159</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>Licenciado</t>
+  </si>
+  <si>
+    <t>Não licenciado</t>
+  </si>
+  <si>
+    <t>[MOS] FM-C2, A4, Fundacao Cearense De Pesquisa E Cultura (10008000590, 322869790), Fortaleza/CE</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (50415723132, 1006703370), Fortaleza/CE</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478453), Fortaleza/CE | [ICAO] TWR 25/40, FORTALEZA | [AISW] SBFZ-COM, TORRE, Pinto Martins</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478453), Fortaleza/CE | [ICAO] APP-U C-150/450, FORTALEZA</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478453), Fortaleza/CE | [ICAO] ACC-U C-261/450, FORTALEZA</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478402), Porto Seguro/BA | [ICAO] ACC-U C-261/450, PORTO SEGURO</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (50415723132, 1007661469), Porto Seguro/BA | [ICAO] ACC-U C-261/450, PORTO SEGURO</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[STEL] L, FA, Comando Da Aeronautica (01020423498, 1002478402), Porto Seguro/BA | [ICAO] ACC-U C-261/450, PORTO SEGURO</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Pendente confirmação</t>
+  </si>
+  <si>
+    <t>Pendente identificação</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>RFeye002159</t>
+  </si>
+  <si>
+    <t>{"Contour":30,"GarbageMask":["mask_Channels.csv","mask_80dBm.csv"],"Persistent":{"ThreadIDList":310,"BrokenMsg":5,"ScansPerMinute":60,"THR1_Global":30,"THR2_OCC":0.1}}</t>
+  </si>
+  <si>
+    <t>matlab.io.ftp.FTP (200.254.11.114:0)
+CONTADOR MÉDIO DE ROMPIMENTO DE MÁSCARA:
+{"beginTime":"01/12/2022 15:07:00","endTime":"01/12/2022 15:12:00","countBroken_Mean":[[300,0],[310,30],[320,0],[330,0],[340,0],[350,0],[360,0],[370,10],[380,0],[390,0]]}
+Não identificadas EMISSÕES PERSISTENTES.</t>
+  </si>
+  <si>
+    <t>01/12/2022 12:04:41</t>
+  </si>
+  <si>
+    <t>01/12/2022 12:12:59</t>
   </si>
 </sst>
 </file>
@@ -602,7 +1445,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -714,11 +1557,29 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
@@ -788,6 +1649,24 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1455,7 +2334,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>119</v>
+        <v>374</v>
       </c>
       <c r="C2" s="4">
         <v>111.90000000000001</v>
@@ -1467,7 +2346,7 @@
         <v>76</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>121</v>
+        <v>377</v>
       </c>
       <c r="G2" s="6">
         <v>-1</v>
@@ -1476,18 +2355,18 @@
         <v>-1</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>125</v>
+        <v>382</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>130</v>
+        <v>388</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>134</v>
+        <v>393</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="M2" s="31">
+        <v>394</v>
+      </c>
+      <c r="M2" s="49">
         <v>44834.518333333333</v>
       </c>
     </row>
@@ -1496,7 +2375,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>119</v>
+        <v>374</v>
       </c>
       <c r="C3" s="4">
         <v>116.5</v>
@@ -1508,7 +2387,7 @@
         <v>100</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>121</v>
+        <v>377</v>
       </c>
       <c r="G3" s="6">
         <v>-1</v>
@@ -1517,18 +2396,18 @@
         <v>-1</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>126</v>
+        <v>383</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>131</v>
+        <v>389</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>134</v>
+        <v>393</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="M3" s="31">
+        <v>394</v>
+      </c>
+      <c r="M3" s="49">
         <v>44834.518333333333</v>
       </c>
     </row>
@@ -1537,7 +2416,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>119</v>
+        <v>374</v>
       </c>
       <c r="C4" s="4">
         <v>127.75</v>
@@ -1549,7 +2428,7 @@
         <v>76</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>122</v>
+        <v>378</v>
       </c>
       <c r="G4" s="6">
         <v>507</v>
@@ -1558,18 +2437,18 @@
         <v>1007661442</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>127</v>
+        <v>384</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>131</v>
+        <v>389</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>134</v>
+        <v>393</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="M4" s="31">
+        <v>394</v>
+      </c>
+      <c r="M4" s="49">
         <v>44834.518333333333</v>
       </c>
     </row>
@@ -1578,7 +2457,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>120</v>
+        <v>375</v>
       </c>
       <c r="C5" s="4">
         <v>110.27500000000001</v>
@@ -1590,7 +2469,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>123</v>
+        <v>379</v>
       </c>
       <c r="G5" s="6">
         <v>-1</v>
@@ -1599,18 +2478,18 @@
         <v>-1</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>128</v>
+        <v>385</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>132</v>
+        <v>390</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>134</v>
+        <v>393</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="M5" s="31">
+        <v>394</v>
+      </c>
+      <c r="M5" s="49">
         <v>44834.519745370373</v>
       </c>
     </row>
@@ -1619,7 +2498,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>120</v>
+        <v>375</v>
       </c>
       <c r="C6" s="4">
         <v>127.7</v>
@@ -1631,7 +2510,7 @@
         <v>50</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>124</v>
+        <v>380</v>
       </c>
       <c r="G6" s="4">
         <v>19</v>
@@ -1640,24 +2519,61 @@
         <v>1002478453</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>129</v>
+        <v>386</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>133</v>
+        <v>391</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>134</v>
+        <v>393</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="M6" s="31">
+        <v>394</v>
+      </c>
+      <c r="M6" s="49">
         <v>44834.519745370373</v>
       </c>
     </row>
     <row r="7" x14ac:dyDescent="0.25">
-      <c r="L7" s="13"/>
-      <c r="M7" s="19"/>
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="C7" s="4">
+        <v>127.65000000000001</v>
+      </c>
+      <c r="D7" s="4">
+        <v>127.65000000000001</v>
+      </c>
+      <c r="E7" s="4">
+        <v>50</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="G7" s="4">
+        <v>-1</v>
+      </c>
+      <c r="H7" s="4">
+        <v>-1</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>394</v>
+      </c>
+      <c r="M7" s="49">
+        <v>44573.481921296298</v>
+      </c>
     </row>
     <row r="8" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
@@ -3993,7 +4909,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>141</v>
+        <v>400</v>
       </c>
       <c r="C2" s="4">
         <v>107.999</v>
@@ -4008,7 +4924,7 @@
         <v>16</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>142</v>
+        <v>402</v>
       </c>
       <c r="H2" s="4">
         <v>230</v>
@@ -4017,15 +4933,15 @@
         <v>322869790</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>149</v>
+        <v>414</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>157</v>
+        <v>428</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="M2" s="33">
+        <v>440</v>
+      </c>
+      <c r="M2" s="51">
         <v>44834.528900462959</v>
       </c>
     </row>
@@ -4034,7 +4950,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>141</v>
+        <v>400</v>
       </c>
       <c r="C3" s="4">
         <v>123.267</v>
@@ -4049,7 +4965,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>143</v>
+        <v>403</v>
       </c>
       <c r="H3" s="4">
         <v>-1</v>
@@ -4058,15 +4974,15 @@
         <v>-1</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>150</v>
+        <v>415</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>158</v>
+        <v>429</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="M3" s="33">
+        <v>440</v>
+      </c>
+      <c r="M3" s="51">
         <v>44834.528900462959</v>
       </c>
     </row>
@@ -4075,7 +4991,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>141</v>
+        <v>400</v>
       </c>
       <c r="C4" s="4">
         <v>125.133</v>
@@ -4090,7 +5006,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>143</v>
+        <v>403</v>
       </c>
       <c r="H4" s="4">
         <v>-1</v>
@@ -4099,15 +5015,15 @@
         <v>-1</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>150</v>
+        <v>415</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>158</v>
+        <v>429</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="M4" s="33">
+        <v>440</v>
+      </c>
+      <c r="M4" s="51">
         <v>44834.528900462959</v>
       </c>
     </row>
@@ -4116,7 +5032,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>141</v>
+        <v>400</v>
       </c>
       <c r="C5" s="4">
         <v>126.334</v>
@@ -4131,7 +5047,7 @@
         <v>17</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>143</v>
+        <v>403</v>
       </c>
       <c r="H5" s="4">
         <v>-1</v>
@@ -4140,15 +5056,15 @@
         <v>-1</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>150</v>
+        <v>415</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>158</v>
+        <v>429</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="M5" s="33">
+        <v>440</v>
+      </c>
+      <c r="M5" s="51">
         <v>44834.528900462959</v>
       </c>
     </row>
@@ -4157,7 +5073,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>141</v>
+        <v>400</v>
       </c>
       <c r="C6" s="4">
         <v>131.55000000000001</v>
@@ -4172,7 +5088,7 @@
         <v>8</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>144</v>
+        <v>404</v>
       </c>
       <c r="H6" s="4">
         <v>507</v>
@@ -4181,15 +5097,15 @@
         <v>1006703370</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>151</v>
+        <v>416</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>159</v>
+        <v>430</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="M6" s="33">
+        <v>440</v>
+      </c>
+      <c r="M6" s="51">
         <v>44834.528900462959</v>
       </c>
     </row>
@@ -4198,7 +5114,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>141</v>
+        <v>400</v>
       </c>
       <c r="C7" s="4">
         <v>132.98599999999999</v>
@@ -4213,7 +5129,7 @@
         <v>34</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="H7" s="4">
         <v>-1</v>
@@ -4222,15 +5138,15 @@
         <v>-1</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>152</v>
+        <v>417</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>160</v>
+        <v>431</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="M7" s="33">
+        <v>440</v>
+      </c>
+      <c r="M7" s="51">
         <v>44834.528900462959</v>
       </c>
     </row>
@@ -4239,7 +5155,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>141</v>
+        <v>400</v>
       </c>
       <c r="C8" s="4">
         <v>133.48500000000001</v>
@@ -4254,7 +5170,7 @@
         <v>19</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="H8" s="4">
         <v>-1</v>
@@ -4263,15 +5179,15 @@
         <v>-1</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>152</v>
+        <v>417</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>160</v>
+        <v>431</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="M8" s="33">
+        <v>440</v>
+      </c>
+      <c r="M8" s="51">
         <v>44834.528900462959</v>
       </c>
     </row>
@@ -4280,7 +5196,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>141</v>
+        <v>400</v>
       </c>
       <c r="C9" s="4">
         <v>135.233</v>
@@ -4295,7 +5211,7 @@
         <v>17</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="H9" s="4">
         <v>-1</v>
@@ -4304,15 +5220,15 @@
         <v>-1</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>152</v>
+        <v>417</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>160</v>
+        <v>431</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="M9" s="33">
+        <v>440</v>
+      </c>
+      <c r="M9" s="51">
         <v>44834.528900462959</v>
       </c>
     </row>
@@ -4321,7 +5237,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>141</v>
+        <v>400</v>
       </c>
       <c r="C10" s="4">
         <v>136.96199999999999</v>
@@ -4336,7 +5252,7 @@
         <v>4</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>145</v>
+        <v>405</v>
       </c>
       <c r="H10" s="4">
         <v>-1</v>
@@ -4345,15 +5261,15 @@
         <v>-1</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>152</v>
+        <v>417</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>160</v>
+        <v>431</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="M10" s="33">
+        <v>440</v>
+      </c>
+      <c r="M10" s="51">
         <v>44834.528900462959</v>
       </c>
     </row>
@@ -4362,7 +5278,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>141</v>
+        <v>400</v>
       </c>
       <c r="C11" s="4">
         <v>128.99100000000001</v>
@@ -4377,7 +5293,7 @@
         <v>34</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>146</v>
+        <v>406</v>
       </c>
       <c r="H11" s="4">
         <v>19</v>
@@ -4386,15 +5302,15 @@
         <v>1002478453</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>153</v>
+        <v>418</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>161</v>
+        <v>432</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="M11" s="33">
+        <v>440</v>
+      </c>
+      <c r="M11" s="51">
         <v>44834.538055555553</v>
       </c>
     </row>
@@ -4403,7 +5319,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>141</v>
+        <v>400</v>
       </c>
       <c r="C12" s="4">
         <v>131.77500000000001</v>
@@ -4418,7 +5334,7 @@
         <v>20</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>147</v>
+        <v>407</v>
       </c>
       <c r="H12" s="4">
         <v>-1</v>
@@ -4427,15 +5343,15 @@
         <v>-1</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>154</v>
+        <v>419</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>162</v>
+        <v>433</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="M12" s="33">
+        <v>440</v>
+      </c>
+      <c r="M12" s="51">
         <v>44834.538055555553</v>
       </c>
     </row>
@@ -4444,7 +5360,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>141</v>
+        <v>400</v>
       </c>
       <c r="C13" s="4">
         <v>132.99600000000001</v>
@@ -4459,7 +5375,7 @@
         <v>28</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>148</v>
+        <v>408</v>
       </c>
       <c r="H13" s="4">
         <v>19</v>
@@ -4468,15 +5384,15 @@
         <v>1002478453</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>155</v>
+        <v>420</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>163</v>
+        <v>434</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="M13" s="33">
+        <v>440</v>
+      </c>
+      <c r="M13" s="51">
         <v>44834.538055555553</v>
       </c>
     </row>
@@ -4485,7 +5401,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>141</v>
+        <v>400</v>
       </c>
       <c r="C14" s="4">
         <v>133.494</v>
@@ -4500,7 +5416,7 @@
         <v>25</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>148</v>
+        <v>408</v>
       </c>
       <c r="H14" s="4">
         <v>19</v>
@@ -4509,15 +5425,15 @@
         <v>1002478453</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>156</v>
+        <v>421</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>163</v>
+        <v>434</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="M14" s="33">
+        <v>440</v>
+      </c>
+      <c r="M14" s="51">
         <v>44834.538055555553</v>
       </c>
     </row>
@@ -4526,7 +5442,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>141</v>
+        <v>400</v>
       </c>
       <c r="C15" s="4">
         <v>135.24299999999999</v>
@@ -4541,7 +5457,7 @@
         <v>25</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>148</v>
+        <v>408</v>
       </c>
       <c r="H15" s="4">
         <v>19</v>
@@ -4550,61 +5466,468 @@
         <v>1002478453</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>156</v>
+        <v>421</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>163</v>
+        <v>434</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="M15" s="33">
+        <v>440</v>
+      </c>
+      <c r="M15" s="51">
         <v>44834.538055555553</v>
       </c>
     </row>
     <row r="16" x14ac:dyDescent="0.25">
-      <c r="L16" s="13"/>
-      <c r="M16" s="18"/>
+      <c r="A16" s="11">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="C16" s="4">
+        <v>123.794</v>
+      </c>
+      <c r="D16" s="4">
+        <v>123.8</v>
+      </c>
+      <c r="E16" s="4">
+        <v>49</v>
+      </c>
+      <c r="F16" s="4">
+        <v>37</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="H16" s="4">
+        <v>19</v>
+      </c>
+      <c r="I16" s="4">
+        <v>1002478402</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="M16" s="51">
+        <v>44573.48333333333</v>
+      </c>
     </row>
     <row r="17" x14ac:dyDescent="0.25">
-      <c r="L17" s="13"/>
-      <c r="M17" s="18"/>
+      <c r="A17" s="11">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="C17" s="4">
+        <v>125.084</v>
+      </c>
+      <c r="D17" s="4">
+        <v>125.075</v>
+      </c>
+      <c r="E17" s="4">
+        <v>49</v>
+      </c>
+      <c r="F17" s="4">
+        <v>37</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="H17" s="4">
+        <v>-1</v>
+      </c>
+      <c r="I17" s="4">
+        <v>-1</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="M17" s="51">
+        <v>44573.48333333333</v>
+      </c>
     </row>
     <row r="18" x14ac:dyDescent="0.25">
-      <c r="L18" s="13"/>
-      <c r="M18" s="18"/>
+      <c r="A18" s="11">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="C18" s="4">
+        <v>125.982</v>
+      </c>
+      <c r="D18" s="4">
+        <v>125.97499999999999</v>
+      </c>
+      <c r="E18" s="4">
+        <v>49</v>
+      </c>
+      <c r="F18" s="4">
+        <v>14</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="H18" s="4">
+        <v>-1</v>
+      </c>
+      <c r="I18" s="4">
+        <v>-1</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="M18" s="51">
+        <v>44573.48333333333</v>
+      </c>
     </row>
     <row r="19" x14ac:dyDescent="0.25">
-      <c r="L19" s="13"/>
-      <c r="M19" s="18"/>
+      <c r="A19" s="11">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="C19" s="4">
+        <v>128.33699999999999</v>
+      </c>
+      <c r="D19" s="4">
+        <v>128.32499999999999</v>
+      </c>
+      <c r="E19" s="4">
+        <v>49</v>
+      </c>
+      <c r="F19" s="4">
+        <v>25</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="H19" s="4">
+        <v>-1</v>
+      </c>
+      <c r="I19" s="4">
+        <v>-1</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="M19" s="51">
+        <v>44573.48333333333</v>
+      </c>
     </row>
     <row r="20" x14ac:dyDescent="0.25">
-      <c r="L20" s="13"/>
-      <c r="M20" s="18"/>
+      <c r="A20" s="11">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="C20" s="4">
+        <v>133.006</v>
+      </c>
+      <c r="D20" s="4">
+        <v>133</v>
+      </c>
+      <c r="E20" s="4">
+        <v>49</v>
+      </c>
+      <c r="F20" s="4">
+        <v>14</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="H20" s="4">
+        <v>-1</v>
+      </c>
+      <c r="I20" s="4">
+        <v>-1</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="M20" s="51">
+        <v>44573.48333333333</v>
+      </c>
     </row>
     <row r="21" x14ac:dyDescent="0.25">
-      <c r="L21" s="13"/>
-      <c r="M21" s="18"/>
+      <c r="A21" s="11">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="C21" s="4">
+        <v>135.28200000000001</v>
+      </c>
+      <c r="D21" s="4">
+        <v>135.27500000000001</v>
+      </c>
+      <c r="E21" s="4">
+        <v>59</v>
+      </c>
+      <c r="F21" s="4">
+        <v>14</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="H21" s="4">
+        <v>-1</v>
+      </c>
+      <c r="I21" s="4">
+        <v>-1</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="M21" s="51">
+        <v>44573.48333333333</v>
+      </c>
     </row>
     <row r="22" x14ac:dyDescent="0.25">
-      <c r="L22" s="13"/>
-      <c r="M22" s="18"/>
+      <c r="A22" s="11">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="C22" s="4">
+        <v>135.643</v>
+      </c>
+      <c r="D22" s="4">
+        <v>135.65000000000001</v>
+      </c>
+      <c r="E22" s="4">
+        <v>59</v>
+      </c>
+      <c r="F22" s="4">
+        <v>37</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="H22" s="4">
+        <v>507</v>
+      </c>
+      <c r="I22" s="4">
+        <v>1007661469</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="M22" s="51">
+        <v>44573.48333333333</v>
+      </c>
     </row>
     <row r="23" x14ac:dyDescent="0.25">
-      <c r="L23" s="13"/>
-      <c r="M23" s="18"/>
+      <c r="A23" s="11">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="C23" s="4">
+        <v>122.81699999999999</v>
+      </c>
+      <c r="D23" s="4">
+        <v>122.825</v>
+      </c>
+      <c r="E23" s="4">
+        <v>49</v>
+      </c>
+      <c r="F23" s="4">
+        <v>11</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="H23" s="4">
+        <v>-1</v>
+      </c>
+      <c r="I23" s="4">
+        <v>-1</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="M23" s="51">
+        <v>44573.490694444445</v>
+      </c>
     </row>
     <row r="24" x14ac:dyDescent="0.25">
-      <c r="L24" s="13"/>
-      <c r="M24" s="18"/>
+      <c r="A24" s="11">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="C24" s="4">
+        <v>125.093</v>
+      </c>
+      <c r="D24" s="4">
+        <v>125.09999999999999</v>
+      </c>
+      <c r="E24" s="4">
+        <v>49</v>
+      </c>
+      <c r="F24" s="4">
+        <v>25</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="H24" s="4">
+        <v>19</v>
+      </c>
+      <c r="I24" s="4">
+        <v>1002478402</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="M24" s="51">
+        <v>44573.490694444445</v>
+      </c>
     </row>
     <row r="25" x14ac:dyDescent="0.25">
-      <c r="L25" s="13"/>
-      <c r="M25" s="18"/>
+      <c r="A25" s="11">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="C25" s="4">
+        <v>133.01599999999999</v>
+      </c>
+      <c r="D25" s="4">
+        <v>133.02500000000001</v>
+      </c>
+      <c r="E25" s="4">
+        <v>49</v>
+      </c>
+      <c r="F25" s="4">
+        <v>26</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="H25" s="4">
+        <v>-1</v>
+      </c>
+      <c r="I25" s="4">
+        <v>-1</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="M25" s="51">
+        <v>44573.490694444445</v>
+      </c>
     </row>
     <row r="26" x14ac:dyDescent="0.25">
-      <c r="L26" s="13"/>
-      <c r="M26" s="18"/>
+      <c r="A26" s="11">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="C26" s="4">
+        <v>135.63399999999999</v>
+      </c>
+      <c r="D26" s="4">
+        <v>135.625</v>
+      </c>
+      <c r="E26" s="4">
+        <v>59</v>
+      </c>
+      <c r="F26" s="4">
+        <v>24</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="H26" s="4">
+        <v>-1</v>
+      </c>
+      <c r="I26" s="4">
+        <v>-1</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="M26" s="51">
+        <v>44573.490694444445</v>
+      </c>
     </row>
     <row r="27" x14ac:dyDescent="0.25">
       <c r="L27" s="13"/>
@@ -5856,24 +7179,89 @@
       </c>
     </row>
     <row r="8" x14ac:dyDescent="0.25">
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="A8" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="9" x14ac:dyDescent="0.25">
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="A9" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="10" x14ac:dyDescent="0.25">
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="A10" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="11" x14ac:dyDescent="0.25">
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="A11" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="12" x14ac:dyDescent="0.25">
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="A12" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="13" x14ac:dyDescent="0.25">
       <c r="D13" s="8"/>
@@ -13950,7 +15338,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CD6A27-DD71-4485-9A29-06B703490C18}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showGridLines="false" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
@@ -14030,6 +15418,74 @@
       </c>
       <c r="E4" s="4" t="s">
         <v>169</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>